<commit_message>
added bluebutton document details and medications details
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.medication.xlsx
+++ b/docs/StructureDefinition-VA.MHV.medication.xlsx
@@ -610,7 +610,7 @@
 This element is labeled as a modifier because the status contains codes that mark the resource as not currently valid.</t>
   </si>
   <si>
-    <t>final</t>
+    <t>active</t>
   </si>
   <si>
     <t>required</t>
@@ -3668,7 +3668,7 @@
         <v>41</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>40</v>

</xml_diff>